<commit_message>
Changed default delaytime value
</commit_message>
<xml_diff>
--- a/bin/Release/Multi Line Pkg Example.xlsx
+++ b/bin/Release/Multi Line Pkg Example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="20895" windowHeight="9915"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20895" windowHeight="9915" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Lines" sheetId="5" r:id="rId5"/>
     <sheet name="BOMItems" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -309,13 +309,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,6 +489,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -567,6 +572,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -601,6 +607,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -776,15 +783,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I191" sqref="I191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
@@ -795,7 +802,7 @@
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +828,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -840,7 +847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -860,7 +867,7 @@
       </c>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -880,7 +887,7 @@
       </c>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -900,7 +907,7 @@
       </c>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -916,20 +923,20 @@
       </c>
       <c r="E6" s="18">
         <f ca="1">G6+H6</f>
-        <v>39786.291666666664</v>
+        <v>41479.291666666664</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="17">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="H6" s="10">
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -949,7 +956,7 @@
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -969,7 +976,7 @@
       </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -989,7 +996,7 @@
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1005,20 +1012,20 @@
       </c>
       <c r="E10" s="18">
         <f ca="1">G10+H10</f>
-        <v>39786.541666666664</v>
+        <v>41479.541666666664</v>
       </c>
       <c r="F10" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="17">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="H10" s="10">
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1038,7 +1045,7 @@
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1058,7 +1065,7 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1074,20 +1081,20 @@
       </c>
       <c r="E13" s="18">
         <f ca="1">G13+H13</f>
-        <v>39786.541666666664</v>
+        <v>41479.541666666664</v>
       </c>
       <c r="F13" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="17">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="H13" s="10">
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1107,7 +1114,7 @@
       </c>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1127,7 +1134,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1147,7 +1154,7 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1167,7 +1174,7 @@
       </c>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1187,7 +1194,7 @@
       </c>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1203,20 +1210,20 @@
       </c>
       <c r="E19" s="18">
         <f ca="1">G19+H19</f>
-        <v>39786.375</v>
+        <v>41479.375</v>
       </c>
       <c r="F19" t="s">
         <v>35</v>
       </c>
       <c r="G19" s="17">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="H19" s="10">
         <v>0.375</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1236,7 +1243,7 @@
       </c>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1256,7 +1263,7 @@
       </c>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1277,7 +1284,7 @@
       <c r="G22" s="17"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1297,7 +1304,7 @@
       </c>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1317,7 +1324,7 @@
       </c>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1337,7 +1344,7 @@
       </c>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1357,7 +1364,7 @@
       </c>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1377,7 +1384,7 @@
       </c>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1397,7 +1404,7 @@
       </c>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1417,7 +1424,7 @@
       </c>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1443,14 +1450,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" customWidth="1"/>
@@ -1461,7 +1468,7 @@
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
@@ -1484,7 +1491,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1234</v>
       </c>
@@ -1504,7 +1511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1235</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1236</v>
       </c>
@@ -1544,7 +1551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1237</v>
       </c>
@@ -1564,7 +1571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1238</v>
       </c>
@@ -1584,7 +1591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1239</v>
       </c>
@@ -1604,7 +1611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1240</v>
       </c>
@@ -1624,7 +1631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1241</v>
       </c>
@@ -1644,7 +1651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1242</v>
       </c>
@@ -1664,7 +1671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1243</v>
       </c>
@@ -1690,16 +1697,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1734,7 +1741,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>Products!A2</f>
         <v>1234</v>
@@ -1770,7 +1777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>Products!A3</f>
         <v>1235</v>
@@ -1806,7 +1813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>Products!A4</f>
         <v>1236</v>
@@ -1842,7 +1849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>Products!A5</f>
         <v>1237</v>
@@ -1878,7 +1885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>Products!A6</f>
         <v>1238</v>
@@ -1914,7 +1921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>Products!A7</f>
         <v>1239</v>
@@ -1950,7 +1957,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>Products!A8</f>
         <v>1240</v>
@@ -1986,7 +1993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>Products!A9</f>
         <v>1241</v>
@@ -2022,7 +2029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>Products!A10</f>
         <v>1242</v>
@@ -2058,7 +2065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>Products!A11</f>
         <v>1243</v>
@@ -2101,20 +2108,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>61</v>
       </c>
@@ -2134,7 +2141,7 @@
       </c>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -2154,7 +2161,7 @@
       </c>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
@@ -2168,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>48</v>
       </c>
@@ -2182,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
@@ -2196,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>52</v>
       </c>
@@ -2210,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2224,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>55</v>
       </c>
@@ -2238,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>57</v>
       </c>
@@ -2252,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
@@ -2272,14 +2279,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -2289,7 +2296,7 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>73</v>
       </c>
@@ -2315,7 +2322,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2324,28 +2331,28 @@
       </c>
       <c r="C2" s="13">
         <f ca="1">E2+F2</f>
-        <v>39786.041666666664</v>
+        <v>41479.041666666664</v>
       </c>
       <c r="D2" s="13">
         <f ca="1">G2+H2</f>
-        <v>39786.999305555553</v>
+        <v>41479.999305555553</v>
       </c>
       <c r="E2" s="11">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="F2" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G2" s="11">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="H2" s="10">
         <v>0.99930555555555556</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -2354,22 +2361,22 @@
       </c>
       <c r="C3" s="13">
         <f ca="1">E3+F3</f>
-        <v>39786.041666666664</v>
+        <v>41479.041666666664</v>
       </c>
       <c r="D3" s="13">
         <f ca="1">G3+H3</f>
-        <v>39786.999305555553</v>
+        <v>41479.999305555553</v>
       </c>
       <c r="E3" s="11">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="F3" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G3" s="11">
         <f ca="1">TODAY()</f>
-        <v>39786</v>
+        <v>41479</v>
       </c>
       <c r="H3" s="10">
         <v>0.99930555555555556</v>
@@ -2382,14 +2389,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -2398,7 +2405,7 @@
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>

</xml_diff>